<commit_message>
Generalized & consolidated scripts
</commit_message>
<xml_diff>
--- a/data/NC/NC2022-elections-analysis.xlsx
+++ b/data/NC/NC2022-elections-analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/dev/method_eval/data/NC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB451CD-51BC-D24D-92FE-6F2DFA404B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D45E97DE-BF47-B648-94D4-AD75D88D0CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{7357A454-9B64-D04B-9AA4-244A1D27914D}"/>
+    <workbookView xWindow="1120" yWindow="500" windowWidth="27300" windowHeight="16940" xr2:uid="{AC2A7E28-C21D-6246-A58E-377DD932C2B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,13 +40,13 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{8217918E-A560-A64E-9558-598D78CEB8A2}" name="NC2022-elections-analysis" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="1" xr16:uid="{AA3513C8-BAD2-2747-B8E1-1A08DFE4C2B2}" name="NC2022-elections-analysis" type="6" refreshedVersion="8" background="1" saveData="1">
     <textPr codePage="10000" sourceFile="/Users/alecramsay/dev/method_eval/data/NC/NC2022-elections-analysis.csv" comma="1">
       <textFields count="26">
         <textField type="text"/>
         <textField type="text"/>
         <textField type="text"/>
-        <textField type="text"/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>XX</t>
   </si>
@@ -163,9 +163,6 @@
   </si>
   <si>
     <t xml:space="preserve"> composite</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 14</t>
   </si>
   <si>
     <t xml:space="preserve"> P2020</t>
@@ -240,7 +237,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="NC2022-elections-analysis" connectionId="1" xr16:uid="{CA8F333B-6FB9-7249-8DB9-D36677A2D5D0}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="NC2022-elections-analysis" connectionId="1" xr16:uid="{EB628E2C-25A9-0243-9EDE-4D771A3DD39A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -539,7 +536,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABA16E99-0D5B-8A49-8AD8-0EAC0775BC34}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44C347A-6769-1E41-BA49-3D493D0DA666}">
   <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -576,7 +573,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -656,8 +653,8 @@
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>29</v>
+      <c r="D2">
+        <v>14</v>
       </c>
       <c r="E2">
         <v>0.49433300000000002</v>
@@ -734,10 +731,10 @@
         <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="D3">
+        <v>14</v>
       </c>
       <c r="E3">
         <v>0.49314400000000003</v>
@@ -814,10 +811,10 @@
         <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>14</v>
       </c>
       <c r="E4">
         <v>0.48094100000000001</v>
@@ -894,10 +891,10 @@
         <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="D5">
+        <v>14</v>
       </c>
       <c r="E5">
         <v>0.49085200000000001</v>
@@ -974,10 +971,10 @@
         <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="D6">
+        <v>14</v>
       </c>
       <c r="E6">
         <v>0.47044399999999997</v>
@@ -1054,10 +1051,10 @@
         <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="D7">
+        <v>14</v>
       </c>
       <c r="E7">
         <v>0.52287499999999998</v>
@@ -1134,10 +1131,10 @@
         <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="D8">
+        <v>14</v>
       </c>
       <c r="E8">
         <v>0.50124299999999999</v>

</xml_diff>